<commit_message>
Added Reset to Default Settings.  Added 3 effects
Додано три єфекти, та сброс у налаштування за замовчуванням
</commit_message>
<xml_diff>
--- a/FieryLedLampMultilingual/Language.xlsx
+++ b/FieryLedLampMultilingual/Language.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$M$150</definedName>
-    <definedName name="Z_02F08554_2E03_4827_AA05_82E0997FBBA8_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$2:$K$150</definedName>
-    <definedName name="Z_3A6F2CDC_256D_4CA7_B8B0_EE39CA0997D0_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$1:$K$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$M$152</definedName>
+    <definedName name="Z_02F08554_2E03_4827_AA05_82E0997FBBA8_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$2:$K$152</definedName>
+    <definedName name="Z_3A6F2CDC_256D_4CA7_B8B0_EE39CA0997D0_.wvu.FilterData" localSheetId="0" hidden="1">Лист1!$A$1:$K$152</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Фильтр 1" guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Фильтр 2" guid="{02F08554-2E03-4827-AA05-82E0997FBBA8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Фильтр 1" guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="674">
   <si>
     <t>Variable</t>
   </si>
@@ -2016,6 +2016,42 @@
   </si>
   <si>
     <t>Максимальний струм матриці</t>
+  </si>
+  <si>
+    <t>Відновити стандартні налаштування</t>
+  </si>
+  <si>
+    <t>Restore Defaults</t>
+  </si>
+  <si>
+    <t>RESTORE_DEFAULT</t>
+  </si>
+  <si>
+    <t>Przywróć domyślne</t>
+  </si>
+  <si>
+    <t>Restaurar valores por defecto</t>
+  </si>
+  <si>
+    <t>Restaurer les valeurs par défaut</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>Paramètres matériels</t>
+  </si>
+  <si>
+    <t>Configuración de hardware</t>
+  </si>
+  <si>
+    <t>Ustawienia sprzętu</t>
+  </si>
+  <si>
+    <t>Параметри обладнання</t>
+  </si>
+  <si>
+    <t>Hardware Setings</t>
   </si>
 </sst>
 </file>
@@ -2397,11 +2433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB999"/>
+  <dimension ref="A1:AB1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4311,23 +4347,23 @@
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="19" t="str">
-        <f t="shared" ref="H50:H72" si="25">CONCATENATE("""",A50,"""",":","""",B50,"""",",")</f>
+        <f t="shared" ref="H50:H75" si="25">CONCATENATE("""",A50,"""",":","""",B50,"""",",")</f>
         <v>"USE_PASS":"Use a password to access this page",</v>
       </c>
       <c r="I50" s="21" t="str">
-        <f t="shared" ref="I50:I72" si="26">CONCATENATE("""",A50,"""",":","""",C50,"""",",")</f>
+        <f t="shared" ref="I50:I75" si="26">CONCATENATE("""",A50,"""",":","""",C50,"""",",")</f>
         <v>"USE_PASS":"Використовувати пароль для доступу до цієї сторінки",</v>
       </c>
       <c r="J50" s="19" t="str">
-        <f t="shared" ref="J50:J72" si="27">CONCATENATE("""",A50,"""",":","""",D50,"""",",")</f>
+        <f t="shared" ref="J50:J74" si="27">CONCATENATE("""",A50,"""",":","""",D50,"""",",")</f>
         <v>"USE_PASS":"Utilice una contraseña para acceder a esta página",</v>
       </c>
       <c r="K50" s="19" t="str">
-        <f t="shared" ref="K50:K72" si="28">CONCATENATE("""",A50,"""",":","""",E50,"""",",")</f>
+        <f t="shared" ref="K50:K74" si="28">CONCATENATE("""",A50,"""",":","""",E50,"""",",")</f>
         <v>"USE_PASS":"Użyj hasła, aby uzyskać dostęp do tej strony",</v>
       </c>
       <c r="L50" s="22" t="str">
-        <f t="shared" ref="L50:L72" si="29">CONCATENATE("""",A50,"""",":","""",F50,"""",",")</f>
+        <f t="shared" ref="L50:L74" si="29">CONCATENATE("""",A50,"""",":","""",F50,"""",",")</f>
         <v>"USE_PASS":"Utilisez un mot de passe pour accéder à cette page",</v>
       </c>
     </row>
@@ -5192,1338 +5228,1338 @@
         <v>"MATRIX_ORIEN":"Orientation de la matrice",</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+    <row r="72" spans="1:12" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="19" t="s">
-        <v>395</v>
+        <v>668</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>396</v>
+        <v>673</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>661</v>
-      </c>
-      <c r="D72" s="16" t="s">
-        <v>397</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="F72" s="20" t="s">
-        <v>399</v>
+        <v>672</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>671</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>669</v>
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="19" t="str">
         <f t="shared" si="25"/>
-        <v>"MAX_CURRENT":"The maximum matrix current",</v>
+        <v>"HARDWARE":"Hardware Setings",</v>
       </c>
       <c r="I72" s="21" t="str">
         <f t="shared" si="26"/>
-        <v>"MAX_CURRENT":"Максимальний струм матриці",</v>
+        <v>"HARDWARE":"Параметри обладнання",</v>
       </c>
       <c r="J72" s="19" t="str">
         <f t="shared" si="27"/>
-        <v>"MAX_CURRENT":"La corriente de matriz máxima",</v>
+        <v>"HARDWARE":"Configuración de hardware",</v>
       </c>
       <c r="K72" s="19" t="str">
         <f t="shared" si="28"/>
-        <v>"MAX_CURRENT":"Maksymalny prąd matrycy",</v>
+        <v>"HARDWARE":"Ustawienia sprzętu",</v>
       </c>
       <c r="L72" s="22" t="str">
         <f t="shared" si="29"/>
-        <v>"MAX_CURRENT":"Le courant de matrice maximal",</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
+        <v>"HARDWARE":"Paramètres matériels",</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="26" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A73" s="19" t="s">
+        <v>664</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>666</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>665</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>667</v>
+      </c>
       <c r="G73" s="17"/>
-      <c r="H73" s="19"/>
-      <c r="J73" s="19"/>
+      <c r="H73" s="19" t="str">
+        <f t="shared" si="25"/>
+        <v>"RESTORE_DEFAULT":"Restore Defaults",</v>
+      </c>
+      <c r="I73" s="19" t="str">
+        <f t="shared" si="26"/>
+        <v>"RESTORE_DEFAULT":"Відновити стандартні налаштування",</v>
+      </c>
+      <c r="J73" s="19" t="str">
+        <f t="shared" si="27"/>
+        <v>"RESTORE_DEFAULT":"Restaurar valores por defecto",</v>
+      </c>
+      <c r="K73" s="19" t="str">
+        <f t="shared" si="28"/>
+        <v>"RESTORE_DEFAULT":"Przywróć domyślne",</v>
+      </c>
+      <c r="L73" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>"RESTORE_DEFAULT":"Restaurer les valeurs par défaut",</v>
+      </c>
     </row>
     <row r="74" spans="1:12" ht="15.75" customHeight="1">
       <c r="A74" s="19" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>402</v>
+        <v>661</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G74" s="17"/>
       <c r="H74" s="19" t="str">
-        <f t="shared" ref="H74:H116" si="30">CONCATENATE("""",A74,"""",":","""",B74,"""",",")</f>
-        <v>"EFFECT":"Effect",</v>
+        <f t="shared" si="25"/>
+        <v>"MAX_CURRENT":"The maximum matrix current",</v>
       </c>
       <c r="I74" s="21" t="str">
-        <f t="shared" ref="I74:I116" si="31">CONCATENATE("""",A74,"""",":","""",C74,"""",",")</f>
-        <v>"EFFECT":"Ефект",</v>
+        <f t="shared" si="26"/>
+        <v>"MAX_CURRENT":"Максимальний струм матриці",</v>
       </c>
       <c r="J74" s="19" t="str">
-        <f t="shared" ref="J74:J116" si="32">CONCATENATE("""",A74,"""",":","""",D74,"""",",")</f>
-        <v>"EFFECT":"Efecto",</v>
+        <f t="shared" si="27"/>
+        <v>"MAX_CURRENT":"La corriente de matriz máxima",</v>
       </c>
       <c r="K74" s="19" t="str">
-        <f t="shared" ref="K74:K116" si="33">CONCATENATE("""",A74,"""",":","""",E74,"""",",")</f>
-        <v>"EFFECT":"Efekt",</v>
+        <f t="shared" si="28"/>
+        <v>"MAX_CURRENT":"Maksymalny prąd matrycy",</v>
       </c>
       <c r="L74" s="22" t="str">
-        <f t="shared" ref="L74:L116" si="34">CONCATENATE("""",A74,"""",":","""",F74,"""",",")</f>
-        <v>"EFFECT":"Effet",</v>
+        <f t="shared" si="29"/>
+        <v>"MAX_CURRENT":"Le courant de matrice maximal",</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A75" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>411</v>
-      </c>
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
       <c r="G75" s="17"/>
-      <c r="H75" s="19" t="str">
-        <f t="shared" si="30"/>
-        <v>"SEL_EFF_CYCLE":"Select effects for Cycle",</v>
-      </c>
-      <c r="I75" s="21" t="str">
-        <f t="shared" si="31"/>
-        <v>"SEL_EFF_CYCLE":"Вибрати ефекти для Циклу",</v>
-      </c>
-      <c r="J75" s="19" t="str">
-        <f t="shared" si="32"/>
-        <v>"SEL_EFF_CYCLE":"Seleccionar efectos para Ciclo",</v>
-      </c>
-      <c r="K75" s="19" t="str">
-        <f t="shared" si="33"/>
-        <v>"SEL_EFF_CYCLE":"Wybierz efekty dla cyklu",</v>
-      </c>
-      <c r="L75" s="22" t="str">
-        <f t="shared" si="34"/>
-        <v>"SEL_EFF_CYCLE":"Sélectionner les effets pour Cycle",</v>
-      </c>
+      <c r="H75" s="19"/>
+      <c r="J75" s="19"/>
     </row>
     <row r="76" spans="1:12" ht="15.75" customHeight="1">
       <c r="A76" s="19" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="G76" s="17"/>
       <c r="H76" s="19" t="str">
-        <f t="shared" si="30"/>
-        <v>"CYCLE_ON":"Cycle ON",</v>
+        <f t="shared" ref="H76:H118" si="30">CONCATENATE("""",A76,"""",":","""",B76,"""",",")</f>
+        <v>"EFFECT":"Effect",</v>
       </c>
       <c r="I76" s="21" t="str">
-        <f t="shared" si="31"/>
-        <v>"CYCLE_ON":"Вкл. Цикл",</v>
+        <f t="shared" ref="I76:I118" si="31">CONCATENATE("""",A76,"""",":","""",C76,"""",",")</f>
+        <v>"EFFECT":"Ефект",</v>
       </c>
       <c r="J76" s="19" t="str">
-        <f t="shared" si="32"/>
-        <v>"CYCLE_ON":"Ciclo ENCENDIDO",</v>
+        <f t="shared" ref="J76:J118" si="32">CONCATENATE("""",A76,"""",":","""",D76,"""",",")</f>
+        <v>"EFFECT":"Efecto",</v>
       </c>
       <c r="K76" s="19" t="str">
-        <f t="shared" si="33"/>
-        <v>"CYCLE_ON":"Cykl WŁ.",</v>
+        <f t="shared" ref="K76:K118" si="33">CONCATENATE("""",A76,"""",":","""",E76,"""",",")</f>
+        <v>"EFFECT":"Efekt",</v>
       </c>
       <c r="L76" s="22" t="str">
-        <f t="shared" si="34"/>
-        <v>"CYCLE_ON":"Cycle MARCHE",</v>
+        <f t="shared" ref="L76:L118" si="34">CONCATENATE("""",A76,"""",":","""",F76,"""",",")</f>
+        <v>"EFFECT":"Effet",</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" s="19" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="G77" s="17"/>
       <c r="H77" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"EFF_CHANGE_TIME":"Effect change time, sec.",</v>
+        <v>"SEL_EFF_CYCLE":"Select effects for Cycle",</v>
       </c>
       <c r="I77" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"EFF_CHANGE_TIME":"Час зміни ефектів, сек.",</v>
+        <v>"SEL_EFF_CYCLE":"Вибрати ефекти для Циклу",</v>
       </c>
       <c r="J77" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"EFF_CHANGE_TIME":"Tiempo de cambio de efecto, seg.",</v>
+        <v>"SEL_EFF_CYCLE":"Seleccionar efectos para Ciclo",</v>
       </c>
       <c r="K77" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"EFF_CHANGE_TIME":"Czas zmiany efektu, sek.",</v>
+        <v>"SEL_EFF_CYCLE":"Wybierz efekty dla cyklu",</v>
       </c>
       <c r="L77" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"EFF_CHANGE_TIME":"Temps de changement d'effet, sec.",</v>
+        <v>"SEL_EFF_CYCLE":"Sélectionner les effets pour Cycle",</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" s="19" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="D78" s="23" t="s">
-        <v>427</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>428</v>
-      </c>
-      <c r="F78" s="23" t="s">
-        <v>429</v>
+        <v>414</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>417</v>
       </c>
       <c r="G78" s="17"/>
       <c r="H78" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"RANDOM_TIME":"+ random time to ... sec.",</v>
+        <v>"CYCLE_ON":"Cycle ON",</v>
       </c>
       <c r="I78" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"RANDOM_TIME":"+ випадковий час до ... сек.",</v>
+        <v>"CYCLE_ON":"Вкл. Цикл",</v>
       </c>
       <c r="J78" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"RANDOM_TIME":". + tiempo aleatorio hasta ... seg.",</v>
+        <v>"CYCLE_ON":"Ciclo ENCENDIDO",</v>
       </c>
       <c r="K78" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"RANDOM_TIME":".+ losowy czas do ... sek.",</v>
+        <v>"CYCLE_ON":"Cykl WŁ.",</v>
       </c>
       <c r="L78" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"RANDOM_TIME":". + temps aléatoire à ... sec.",</v>
+        <v>"CYCLE_ON":"Cycle MARCHE",</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" s="19" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="D79" s="16" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>435</v>
+        <v>422</v>
+      </c>
+      <c r="F79" s="20" t="s">
+        <v>423</v>
       </c>
       <c r="G79" s="17"/>
       <c r="H79" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"MIX_EFF":"Mix selected effects",</v>
+        <v>"EFF_CHANGE_TIME":"Effect change time, sec.",</v>
       </c>
       <c r="I79" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"MIX_EFF":"Перемішати вибрані ефекти",</v>
+        <v>"EFF_CHANGE_TIME":"Час зміни ефектів, сек.",</v>
       </c>
       <c r="J79" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"MIX_EFF":"Mezclar efectos seleccionados",</v>
+        <v>"EFF_CHANGE_TIME":"Tiempo de cambio de efecto, seg.",</v>
       </c>
       <c r="K79" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"MIX_EFF":"Wymieszaj wybrane efekty",</v>
+        <v>"EFF_CHANGE_TIME":"Czas zmiany efektu, sek.",</v>
       </c>
       <c r="L79" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"MIX_EFF":"Mélanger les effets sélectionnés",</v>
+        <v>"EFF_CHANGE_TIME":"Temps de changement d'effet, sec.",</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" s="19" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>438</v>
-      </c>
-      <c r="D80" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="E80" s="16" t="s">
-        <v>440</v>
-      </c>
-      <c r="F80" s="20" t="s">
-        <v>441</v>
+        <v>426</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>427</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>428</v>
+      </c>
+      <c r="F80" s="23" t="s">
+        <v>429</v>
       </c>
       <c r="G80" s="17"/>
       <c r="H80" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"RANDOM_EFF_PARAM":"Random selection of effects parameters",</v>
+        <v>"RANDOM_TIME":"+ random time to ... sec.",</v>
       </c>
       <c r="I80" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"RANDOM_EFF_PARAM":"Випадковий вибір параметрів ефектів",</v>
+        <v>"RANDOM_TIME":"+ випадковий час до ... сек.",</v>
       </c>
       <c r="J80" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"RANDOM_EFF_PARAM":"Selección aleatoria de parámetros de efectos",</v>
+        <v>"RANDOM_TIME":". + tiempo aleatorio hasta ... seg.",</v>
       </c>
       <c r="K80" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"RANDOM_EFF_PARAM":"Losowy wybór parametrów efektów",</v>
+        <v>"RANDOM_TIME":".+ losowy czas do ... sek.",</v>
       </c>
       <c r="L80" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"RANDOM_EFF_PARAM":"Sélection aléatoire des paramètres d'effets",</v>
+        <v>"RANDOM_TIME":". + temps aléatoire à ... sec.",</v>
       </c>
     </row>
     <row r="81" spans="1:12" ht="15.75" customHeight="1">
       <c r="A81" s="19" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>446</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>447</v>
+        <v>434</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>435</v>
       </c>
       <c r="G81" s="17"/>
       <c r="H81" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"ON_CYCLE_AFTER_RESTART":"Enable Cycle after lamp restart",</v>
+        <v>"MIX_EFF":"Mix selected effects",</v>
       </c>
       <c r="I81" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"ON_CYCLE_AFTER_RESTART":"Увімк. Цикл після перезапуску лампи",</v>
+        <v>"MIX_EFF":"Перемішати вибрані ефекти",</v>
       </c>
       <c r="J81" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"ON_CYCLE_AFTER_RESTART":"Habilitar ciclo después de reiniciar la lámpara",</v>
+        <v>"MIX_EFF":"Mezclar efectos seleccionados",</v>
       </c>
       <c r="K81" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"ON_CYCLE_AFTER_RESTART":"Włącz cykl po ponownym uruchomieniu lampy",</v>
+        <v>"MIX_EFF":"Wymieszaj wybrane efekty",</v>
       </c>
       <c r="L81" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"ON_CYCLE_AFTER_RESTART":"Activer le cycle après le redémarrage de la lampe",</v>
+        <v>"MIX_EFF":"Mélanger les effets sélectionnés",</v>
       </c>
     </row>
     <row r="82" spans="1:12" ht="15.75" customHeight="1">
       <c r="A82" s="19" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="D82" s="16" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="G82" s="17"/>
       <c r="H82" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"BUTTON_ONLY_CYCLE_EFF":"Button - only the effects selected in the Cycle",</v>
+        <v>"RANDOM_EFF_PARAM":"Random selection of effects parameters",</v>
       </c>
       <c r="I82" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"BUTTON_ONLY_CYCLE_EFF":"Кнопкою - лише ефекти, вибрані в Циклі",</v>
+        <v>"RANDOM_EFF_PARAM":"Випадковий вибір параметрів ефектів",</v>
       </c>
       <c r="J82" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"BUTTON_ONLY_CYCLE_EFF":"Botón - solo los efectos seleccionados en el Ciclo",</v>
+        <v>"RANDOM_EFF_PARAM":"Selección aleatoria de parámetros de efectos",</v>
       </c>
       <c r="K82" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"BUTTON_ONLY_CYCLE_EFF":"Przycisk - tylko efekty wybrane w Cyklu",</v>
+        <v>"RANDOM_EFF_PARAM":"Losowy wybór parametrów efektów",</v>
       </c>
       <c r="L82" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"BUTTON_ONLY_CYCLE_EFF":"Bouton - uniquement les effets sélectionnés dans le Cycle",</v>
+        <v>"RANDOM_EFF_PARAM":"Sélection aléatoire des paramètres d'effets",</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="15.75" customHeight="1">
       <c r="A83" s="19" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="E83" s="16" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="G83" s="17"/>
       <c r="H83" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"ORIGINAL_STATE_EFF":"Resetting effects settings to their original state",</v>
+        <v>"ON_CYCLE_AFTER_RESTART":"Enable Cycle after lamp restart",</v>
       </c>
       <c r="I83" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"ORIGINAL_STATE_EFF":"Скидання налаштувань ефектів у початкові",</v>
+        <v>"ON_CYCLE_AFTER_RESTART":"Увімк. Цикл після перезапуску лампи",</v>
       </c>
       <c r="J83" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"ORIGINAL_STATE_EFF":"Restablecimiento de la configuración de efectos a su estado original",</v>
+        <v>"ON_CYCLE_AFTER_RESTART":"Habilitar ciclo después de reiniciar la lámpara",</v>
       </c>
       <c r="K83" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"ORIGINAL_STATE_EFF":"Resetowanie ustawień efektów do ich pierwotnego stanu",</v>
+        <v>"ON_CYCLE_AFTER_RESTART":"Włącz cykl po ponownym uruchomieniu lampy",</v>
       </c>
       <c r="L83" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"ORIGINAL_STATE_EFF":"Réinitialisation des paramètres d'effets à leur état d'origine",</v>
+        <v>"ON_CYCLE_AFTER_RESTART":"Activer le cycle après le redémarrage de la lampe",</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="15.75" customHeight="1">
       <c r="A84" s="19" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="G84" s="17"/>
       <c r="H84" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"SAVE_EFF_TO_FILE":"Save effects settings to a file",</v>
+        <v>"BUTTON_ONLY_CYCLE_EFF":"Button - only the effects selected in the Cycle",</v>
       </c>
       <c r="I84" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"SAVE_EFF_TO_FILE":"Зберегти налаштування ефектів у файл",</v>
+        <v>"BUTTON_ONLY_CYCLE_EFF":"Кнопкою - лише ефекти, вибрані в Циклі",</v>
       </c>
       <c r="J84" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"SAVE_EFF_TO_FILE":"Guardar ajustes de efectos en un archivo",</v>
+        <v>"BUTTON_ONLY_CYCLE_EFF":"Botón - solo los efectos seleccionados en el Ciclo",</v>
       </c>
       <c r="K84" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"SAVE_EFF_TO_FILE":"Zapisz ustawienia efektów do pliku",</v>
+        <v>"BUTTON_ONLY_CYCLE_EFF":"Przycisk - tylko efekty wybrane w Cyklu",</v>
       </c>
       <c r="L84" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"SAVE_EFF_TO_FILE":"Enregistrer les paramètres d'effets dans un fichier",</v>
+        <v>"BUTTON_ONLY_CYCLE_EFF":"Bouton - uniquement les effets sélectionnés dans le Cycle",</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="15.75" customHeight="1">
       <c r="A85" s="19" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="D85" s="16" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"READ_EFF_FROM_FILE":"Read effect settings from a file",</v>
+        <v>"ORIGINAL_STATE_EFF":"Resetting effects settings to their original state",</v>
       </c>
       <c r="I85" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"READ_EFF_FROM_FILE":"Читати налаштування ефектів із файлу",</v>
+        <v>"ORIGINAL_STATE_EFF":"Скидання налаштувань ефектів у початкові",</v>
       </c>
       <c r="J85" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"READ_EFF_FROM_FILE":"Leer ajustes de efectos desde un archivo",</v>
+        <v>"ORIGINAL_STATE_EFF":"Restablecimiento de la configuración de efectos a su estado original",</v>
       </c>
       <c r="K85" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"READ_EFF_FROM_FILE":"Odczytaj ustawienia efektów z pliku",</v>
+        <v>"ORIGINAL_STATE_EFF":"Resetowanie ustawień efektów do ich pierwotnego stanu",</v>
       </c>
       <c r="L85" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"READ_EFF_FROM_FILE":"Lire les paramètres d'effet à partir d'un fichier",</v>
+        <v>"ORIGINAL_STATE_EFF":"Réinitialisation des paramètres d'effets à leur état d'origine",</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="15.75" customHeight="1">
       <c r="A86" s="19" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="D86" s="16" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="G86" s="17"/>
       <c r="H86" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"RUN_TEXT":"Running line text",</v>
+        <v>"SAVE_EFF_TO_FILE":"Save effects settings to a file",</v>
       </c>
       <c r="I86" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"RUN_TEXT":"Текст рядка, що біжить",</v>
+        <v>"SAVE_EFF_TO_FILE":"Зберегти налаштування ефектів у файл",</v>
       </c>
       <c r="J86" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"RUN_TEXT":"Texto de línea continua",</v>
+        <v>"SAVE_EFF_TO_FILE":"Guardar ajustes de efectos en un archivo",</v>
       </c>
       <c r="K86" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"RUN_TEXT":"Uruchomiony tekst linii",</v>
+        <v>"SAVE_EFF_TO_FILE":"Zapisz ustawienia efektów do pliku",</v>
       </c>
       <c r="L86" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"RUN_TEXT":"Texte en ligne courant",</v>
+        <v>"SAVE_EFF_TO_FILE":"Enregistrer les paramètres d'effets dans un fichier",</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="15.75" customHeight="1">
       <c r="A87" s="19" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="G87" s="17"/>
       <c r="H87" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"PERIOD_RUN_TIME":"Periodicity of time output in a line 0-60 min. 0 - do not display time",</v>
+        <v>"READ_EFF_FROM_FILE":"Read effect settings from a file",</v>
       </c>
       <c r="I87" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"PERIOD_RUN_TIME":"Періодичність виведення часу рядком 0-60 хв. 0 - не виводити час",</v>
+        <v>"READ_EFF_FROM_FILE":"Читати налаштування ефектів із файлу",</v>
       </c>
       <c r="J87" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"PERIOD_RUN_TIME":"Periodicidad de salida de tiempo en una línea 0-60 min. 0 - no muestra la hora",</v>
+        <v>"READ_EFF_FROM_FILE":"Leer ajustes de efectos desde un archivo",</v>
       </c>
       <c r="K87" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"PERIOD_RUN_TIME":"Częstotliwość czasu wyprowadzania w linii 0-60 min. 0 - nie wyświetlaj czasu",</v>
+        <v>"READ_EFF_FROM_FILE":"Odczytaj ustawienia efektów z pliku",</v>
       </c>
       <c r="L87" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"PERIOD_RUN_TIME":"Périodicité de sortie de temps dans une ligne 0-60 min. 0 - ne pas afficher l'heure",</v>
+        <v>"READ_EFF_FROM_FILE":"Lire les paramètres d'effet à partir d'un fichier",</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="15.75" customHeight="1">
       <c r="A88" s="19" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E88" s="16" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="G88" s="17"/>
       <c r="H88" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"DISPLAY_TIME_LAMP_OFF":"Display the time on a switched-off lamp",</v>
+        <v>"RUN_TEXT":"Running line text",</v>
       </c>
       <c r="I88" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"DISPLAY_TIME_LAMP_OFF":"Виводити час на вимкненій лампі",</v>
+        <v>"RUN_TEXT":"Текст рядка, що біжить",</v>
       </c>
       <c r="J88" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"DISPLAY_TIME_LAMP_OFF":"Mostrar la hora en una lámpara apagada",</v>
+        <v>"RUN_TEXT":"Texto de línea continua",</v>
       </c>
       <c r="K88" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"DISPLAY_TIME_LAMP_OFF":"Wyświetlaj czas na wyłączonej lampie",</v>
+        <v>"RUN_TEXT":"Uruchomiony tekst linii",</v>
       </c>
       <c r="L88" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"DISPLAY_TIME_LAMP_OFF":"Afficher l'heure sur une lampe éteinte",</v>
+        <v>"RUN_TEXT":"Texte en ligne courant",</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="15.75" customHeight="1">
       <c r="A89" s="19" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="D89" s="16" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="G89" s="17"/>
       <c r="H89" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"HOUR_OF_NIGHT":"Hour of transition to night time",</v>
+        <v>"PERIOD_RUN_TIME":"Periodicity of time output in a line 0-60 min. 0 - do not display time",</v>
       </c>
       <c r="I89" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"HOUR_OF_NIGHT":"Година переходу на нічний час",</v>
+        <v>"PERIOD_RUN_TIME":"Періодичність виведення часу рядком 0-60 хв. 0 - не виводити час",</v>
       </c>
       <c r="J89" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"HOUR_OF_NIGHT":"Hora de transición a la noche",</v>
+        <v>"PERIOD_RUN_TIME":"Periodicidad de salida de tiempo en una línea 0-60 min. 0 - no muestra la hora",</v>
       </c>
       <c r="K89" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"HOUR_OF_NIGHT":"Godzina przejścia na porę nocną",</v>
+        <v>"PERIOD_RUN_TIME":"Częstotliwość czasu wyprowadzania w linii 0-60 min. 0 - nie wyświetlaj czasu",</v>
       </c>
       <c r="L89" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"HOUR_OF_NIGHT":"Heure de passage à la nuit",</v>
+        <v>"PERIOD_RUN_TIME":"Périodicité de sortie de temps dans une ligne 0-60 min. 0 - ne pas afficher l'heure",</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="15.75" customHeight="1">
       <c r="A90" s="19" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="D90" s="16" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="E90" s="16" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="G90" s="17"/>
       <c r="H90" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"BR_NIGHT":"Brightness at night",</v>
+        <v>"DISPLAY_TIME_LAMP_OFF":"Display the time on a switched-off lamp",</v>
       </c>
       <c r="I90" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"BR_NIGHT":"Яскравість у нічний час",</v>
+        <v>"DISPLAY_TIME_LAMP_OFF":"Виводити час на вимкненій лампі",</v>
       </c>
       <c r="J90" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"BR_NIGHT":"Brillo en la noche",</v>
+        <v>"DISPLAY_TIME_LAMP_OFF":"Mostrar la hora en una lámpara apagada",</v>
       </c>
       <c r="K90" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"BR_NIGHT":"Jasność w nocy",</v>
+        <v>"DISPLAY_TIME_LAMP_OFF":"Wyświetlaj czas na wyłączonej lampie",</v>
       </c>
       <c r="L90" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"BR_NIGHT":"Luminosité la nuit",</v>
+        <v>"DISPLAY_TIME_LAMP_OFF":"Afficher l'heure sur une lampe éteinte",</v>
       </c>
     </row>
     <row r="91" spans="1:12" ht="15.75" customHeight="1">
       <c r="A91" s="19" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="C91" s="19" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="D91" s="16" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="G91" s="17"/>
       <c r="H91" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"VOICE_TIME_NIGHT":"Voice the time at night",</v>
+        <v>"HOUR_OF_NIGHT":"Hour of transition to night time",</v>
       </c>
       <c r="I91" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"VOICE_TIME_NIGHT":"Озвучувати час уночі",</v>
+        <v>"HOUR_OF_NIGHT":"Година переходу на нічний час",</v>
       </c>
       <c r="J91" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"VOICE_TIME_NIGHT":"Voz el tiempo en la noche",</v>
+        <v>"HOUR_OF_NIGHT":"Hora de transición a la noche",</v>
       </c>
       <c r="K91" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"VOICE_TIME_NIGHT":"Wypowiadaj czas w nocy",</v>
+        <v>"HOUR_OF_NIGHT":"Godzina przejścia na porę nocną",</v>
       </c>
       <c r="L91" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"VOICE_TIME_NIGHT":"Exprimez l'heure la nuit",</v>
+        <v>"HOUR_OF_NIGHT":"Heure de passage à la nuit",</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="15.75" customHeight="1">
       <c r="A92" s="19" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="G92" s="17"/>
       <c r="H92" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"SOUND_VOLUM":"The volume of sounding",</v>
+        <v>"BR_NIGHT":"Brightness at night",</v>
       </c>
       <c r="I92" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"SOUND_VOLUM":"Гучність озвучування",</v>
+        <v>"BR_NIGHT":"Яскравість у нічний час",</v>
       </c>
       <c r="J92" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"SOUND_VOLUM":"El volumen de sonido",</v>
+        <v>"BR_NIGHT":"Brillo en la noche",</v>
       </c>
       <c r="K92" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"SOUND_VOLUM":"Głośność brzmienia",</v>
+        <v>"BR_NIGHT":"Jasność w nocy",</v>
       </c>
       <c r="L92" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"SOUND_VOLUM":"Le volume sonore",</v>
+        <v>"BR_NIGHT":"Luminosité la nuit",</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="15.75" customHeight="1">
       <c r="A93" s="19" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="G93" s="17"/>
       <c r="H93" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"HOUR_OF_DAY":"Hour of transition to day time",</v>
+        <v>"VOICE_TIME_NIGHT":"Voice the time at night",</v>
       </c>
       <c r="I93" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"HOUR_OF_DAY":"Година переходу на денний час",</v>
+        <v>"VOICE_TIME_NIGHT":"Озвучувати час уночі",</v>
       </c>
       <c r="J93" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"HOUR_OF_DAY":"Hora de transición a la hora del día",</v>
+        <v>"VOICE_TIME_NIGHT":"Voz el tiempo en la noche",</v>
       </c>
       <c r="K93" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"HOUR_OF_DAY":"Godzina przejścia na czas dzienny",</v>
+        <v>"VOICE_TIME_NIGHT":"Wypowiadaj czas w nocy",</v>
       </c>
       <c r="L93" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"HOUR_OF_DAY":"Heure de passage à l'heure de jour",</v>
+        <v>"VOICE_TIME_NIGHT":"Exprimez l'heure la nuit",</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="15.75" customHeight="1">
       <c r="A94" s="19" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="G94" s="17"/>
       <c r="H94" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"BR_DAY":"Brightness during the day",</v>
+        <v>"SOUND_VOLUM":"The volume of sounding",</v>
       </c>
       <c r="I94" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"BR_DAY":"Яскравість у денний час",</v>
+        <v>"SOUND_VOLUM":"Гучність озвучування",</v>
       </c>
       <c r="J94" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"BR_DAY":"Brillo durante el día",</v>
+        <v>"SOUND_VOLUM":"El volumen de sonido",</v>
       </c>
       <c r="K94" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"BR_DAY":"Jasność w ciągu dnia",</v>
+        <v>"SOUND_VOLUM":"Głośność brzmienia",</v>
       </c>
       <c r="L94" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"BR_DAY":"Luminosité pendant la journée",</v>
+        <v>"SOUND_VOLUM":"Le volume sonore",</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="15.75" customHeight="1">
       <c r="A95" s="19" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="D95" s="16" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="G95" s="17"/>
       <c r="H95" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"VOICE_TIME_DAY":"Voice the time of day",</v>
+        <v>"HOUR_OF_DAY":"Hour of transition to day time",</v>
       </c>
       <c r="I95" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"VOICE_TIME_DAY":"Озвучувати час вдень",</v>
+        <v>"HOUR_OF_DAY":"Година переходу на денний час",</v>
       </c>
       <c r="J95" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"VOICE_TIME_DAY":"Voz de la hora del día",</v>
+        <v>"HOUR_OF_DAY":"Hora de transición a la hora del día",</v>
       </c>
       <c r="K95" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"VOICE_TIME_DAY":"Wypowiedz porę dnia",</v>
+        <v>"HOUR_OF_DAY":"Godzina przejścia na czas dzienny",</v>
       </c>
       <c r="L95" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"VOICE_TIME_DAY":"Voix de l'heure du jour",</v>
+        <v>"HOUR_OF_DAY":"Heure de passage à l'heure de jour",</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="15.75" customHeight="1">
       <c r="A96" s="19" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="G96" s="17"/>
       <c r="H96" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"TIMER_ON_OFF":"Timer on/off of Lamp",</v>
+        <v>"BR_DAY":"Brightness during the day",</v>
       </c>
       <c r="I96" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"TIMER_ON_OFF":"Таймер вкл / відкл лампы.",</v>
+        <v>"BR_DAY":"Яскравість у денний час",</v>
       </c>
       <c r="J96" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"TIMER_ON_OFF":"Temporizador de encendido/apagado de la lámpara",</v>
+        <v>"BR_DAY":"Brillo durante el día",</v>
       </c>
       <c r="K96" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"TIMER_ON_OFF":"Włącznik/wyłącznik czasowy lampy",</v>
+        <v>"BR_DAY":"Jasność w ciągu dnia",</v>
       </c>
       <c r="L96" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"TIMER_ON_OFF":"Minuterie marche/arrêt de la lampe",</v>
+        <v>"BR_DAY":"Luminosité pendant la journée",</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="15.75" customHeight="1">
       <c r="A97" s="19" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>540</v>
-      </c>
-      <c r="D97" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="E97" s="20" t="s">
-        <v>542</v>
+        <v>528</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>530</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="G97" s="17"/>
       <c r="H97" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"TIMER_RUN":" 'Run': 'Runing'",</v>
+        <v>"VOICE_TIME_DAY":"Voice the time of day",</v>
       </c>
       <c r="I97" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"TIMER_RUN":"'Запустити':'Запущено'",</v>
+        <v>"VOICE_TIME_DAY":"Озвучувати час вдень",</v>
       </c>
       <c r="J97" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"TIMER_RUN":" 'Correr': 'Lanzado'",</v>
+        <v>"VOICE_TIME_DAY":"Voz de la hora del día",</v>
       </c>
       <c r="K97" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"TIMER_RUN":" 'Uruchomić': 'Uruchomiona'",</v>
+        <v>"VOICE_TIME_DAY":"Wypowiedz porę dnia",</v>
       </c>
       <c r="L97" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"TIMER_RUN":" 'Courir' : 'Lancé'",</v>
+        <v>"VOICE_TIME_DAY":"Voix de l'heure du jour",</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="15.75" customHeight="1">
       <c r="A98" s="19" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="F98" s="20" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="G98" s="17"/>
       <c r="H98" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"BUTTON_ACTIVE":"The button is activated",</v>
+        <v>"TIMER_ON_OFF":"Timer on/off of Lamp",</v>
       </c>
       <c r="I98" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"BUTTON_ACTIVE":"Кнопка активована",</v>
+        <v>"TIMER_ON_OFF":"Таймер вкл / відкл лампы.",</v>
       </c>
       <c r="J98" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"BUTTON_ACTIVE":"El botón está activado",</v>
+        <v>"TIMER_ON_OFF":"Temporizador de encendido/apagado de la lámpara",</v>
       </c>
       <c r="K98" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"BUTTON_ACTIVE":"Przycisk jest aktywny",</v>
+        <v>"TIMER_ON_OFF":"Włącznik/wyłącznik czasowy lampy",</v>
       </c>
       <c r="L98" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"BUTTON_ACTIVE":"Le bouton est activé",</v>
+        <v>"TIMER_ON_OFF":"Minuterie marche/arrêt de la lampe",</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="15.75" customHeight="1">
       <c r="A99" s="19" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>552</v>
-      </c>
-      <c r="D99" s="16" t="s">
-        <v>553</v>
-      </c>
-      <c r="E99" s="16" t="s">
-        <v>554</v>
+        <v>540</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>541</v>
+      </c>
+      <c r="E99" s="20" t="s">
+        <v>542</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="G99" s="17"/>
       <c r="H99" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"POWER_FAILURE":"Do not turn on after power failure",</v>
+        <v>"TIMER_RUN":" 'Run': 'Runing'",</v>
       </c>
       <c r="I99" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"POWER_FAILURE":"Не включати після знеструмлення",</v>
+        <v>"TIMER_RUN":"'Запустити':'Запущено'",</v>
       </c>
       <c r="J99" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"POWER_FAILURE":"No encender después de un corte de energía",</v>
+        <v>"TIMER_RUN":" 'Correr': 'Lanzado'",</v>
       </c>
       <c r="K99" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"POWER_FAILURE":"Nie włączaj po awarii zasilania",</v>
+        <v>"TIMER_RUN":" 'Uruchomić': 'Uruchomiona'",</v>
       </c>
       <c r="L99" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"POWER_FAILURE":"Ne pas allumer après une panne de courant",</v>
+        <v>"TIMER_RUN":" 'Courir' : 'Lancé'",</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="15.75" customHeight="1">
       <c r="A100" s="19" t="s">
-        <v>556</v>
+        <v>544</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>557</v>
+        <v>545</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="G100" s="17"/>
       <c r="H100" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"DARK_THEME":"Dark theme",</v>
+        <v>"BUTTON_ACTIVE":"The button is activated",</v>
       </c>
       <c r="I100" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"DARK_THEME":"Темна тема",</v>
+        <v>"BUTTON_ACTIVE":"Кнопка активована",</v>
       </c>
       <c r="J100" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"DARK_THEME":"tema oscuro",</v>
+        <v>"BUTTON_ACTIVE":"El botón está activado",</v>
       </c>
       <c r="K100" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"DARK_THEME":"ciemny schemat",</v>
+        <v>"BUTTON_ACTIVE":"Przycisk jest aktywny",</v>
       </c>
       <c r="L100" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"DARK_THEME":"Thème sombre",</v>
+        <v>"BUTTON_ACTIVE":"Le bouton est activé",</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="15.75" customHeight="1">
       <c r="A101" s="19" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
       <c r="G101" s="17"/>
       <c r="H101" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"AUTO_TIMER":"Automatic lamp shutdown timer (for the forgetful)",</v>
+        <v>"POWER_FAILURE":"Do not turn on after power failure",</v>
       </c>
       <c r="I101" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"AUTO_TIMER":"Автоматичний таймер відключення лампи (для забудькуватих)",</v>
+        <v>"POWER_FAILURE":"Не включати після знеструмлення",</v>
       </c>
       <c r="J101" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"AUTO_TIMER":"Temporizador de apagado automático de la lámpara (para los olvidadizos)",</v>
+        <v>"POWER_FAILURE":"No encender después de un corte de energía",</v>
       </c>
       <c r="K101" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"AUTO_TIMER":"Automatyczny wyłącznik czasowy lampy (dla zapominalskich)",</v>
+        <v>"POWER_FAILURE":"Nie włączaj po awarii zasilania",</v>
       </c>
       <c r="L101" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"AUTO_TIMER":"Minuterie d'arrêt automatique de la lampe (pour les oublieux)",</v>
+        <v>"POWER_FAILURE":"Ne pas allumer après une panne de courant",</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="15.75" customHeight="1">
       <c r="A102" s="19" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="G102" s="17"/>
       <c r="H102" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"NOT_OFF":"Do not turn off",</v>
+        <v>"DARK_THEME":"Dark theme",</v>
       </c>
       <c r="I102" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"NOT_OFF":"Не вимикати",</v>
+        <v>"DARK_THEME":"Темна тема",</v>
       </c>
       <c r="J102" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"NOT_OFF":"No apagar",</v>
+        <v>"DARK_THEME":"tema oscuro",</v>
       </c>
       <c r="K102" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"NOT_OFF":"Nie wyłączać",</v>
+        <v>"DARK_THEME":"ciemny schemat",</v>
       </c>
       <c r="L102" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"NOT_OFF":"Ne pas eteindre",</v>
+        <v>"DARK_THEME":"Thème sombre",</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="15.75" customHeight="1">
       <c r="A103" s="19" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="G103" s="17"/>
       <c r="H103" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"HOURS":"hours",</v>
+        <v>"AUTO_TIMER":"Automatic lamp shutdown timer (for the forgetful)",</v>
       </c>
       <c r="I103" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"HOURS":"годин",</v>
+        <v>"AUTO_TIMER":"Автоматичний таймер відключення лампи (для забудькуватих)",</v>
       </c>
       <c r="J103" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"HOURS":"horas",</v>
+        <v>"AUTO_TIMER":"Temporizador de apagado automático de la lámpara (para los olvidadizos)",</v>
       </c>
       <c r="K103" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"HOURS":"godziny",</v>
+        <v>"AUTO_TIMER":"Automatyczny wyłącznik czasowy lampy (dla zapominalskich)",</v>
       </c>
       <c r="L103" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"HOURS":"heures",</v>
+        <v>"AUTO_TIMER":"Minuterie d'arrêt automatique de la lampe (pour les oublieux)",</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="15.75" customHeight="1">
       <c r="A104" s="19" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="G104" s="17"/>
       <c r="H104" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"HOUR":"hour",</v>
+        <v>"NOT_OFF":"Do not turn off",</v>
       </c>
       <c r="I104" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"HOUR":"година",</v>
+        <v>"NOT_OFF":"Не вимикати",</v>
       </c>
       <c r="J104" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"HOUR":"hora",</v>
+        <v>"NOT_OFF":"No apagar",</v>
       </c>
       <c r="K104" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"HOUR":"godzina",</v>
+        <v>"NOT_OFF":"Nie wyłączać",</v>
       </c>
       <c r="L104" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"HOUR":"heure",</v>
+        <v>"NOT_OFF":"Ne pas eteindre",</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="15.75" customHeight="1">
       <c r="A105" s="19" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="B105" s="19" t="s">
         <v>575</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="D105" s="16" t="s">
         <v>577</v>
@@ -6537,551 +6573,631 @@
       <c r="G105" s="17"/>
       <c r="H105" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"HOURS2":"hours",</v>
+        <v>"HOURS":"hours",</v>
       </c>
       <c r="I105" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"HOURS2":"години",</v>
+        <v>"HOURS":"годин",</v>
       </c>
       <c r="J105" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"HOURS2":"horas",</v>
+        <v>"HOURS":"horas",</v>
       </c>
       <c r="K105" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"HOURS2":"godziny",</v>
+        <v>"HOURS":"godziny",</v>
       </c>
       <c r="L105" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"HOURS2":"heures",</v>
+        <v>"HOURS":"heures",</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="15.75" customHeight="1">
       <c r="A106" s="19" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="G106" s="17"/>
       <c r="H106" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"CONTROL_SEVERAL_LAMPS":"Control of several lamps",</v>
+        <v>"HOUR":"hour",</v>
       </c>
       <c r="I106" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"CONTROL_SEVERAL_LAMPS":"Управління кількома лампами",</v>
+        <v>"HOUR":"година",</v>
       </c>
       <c r="J106" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"CONTROL_SEVERAL_LAMPS":"Control de varias lámparas",</v>
+        <v>"HOUR":"hora",</v>
       </c>
       <c r="K106" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"CONTROL_SEVERAL_LAMPS":"Sterowanie kilkoma lampami",</v>
+        <v>"HOUR":"godzina",</v>
       </c>
       <c r="L106" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"CONTROL_SEVERAL_LAMPS":"Commande de plusieurs lampes",</v>
+        <v>"HOUR":"heure",</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="15.75" customHeight="1">
       <c r="A107" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="G107" s="17"/>
       <c r="H107" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"SOUND_EFF_SET":"Sound effects settings",</v>
+        <v>"HOURS2":"hours",</v>
       </c>
       <c r="I107" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"SOUND_EFF_SET":"Налаштування озвучування ефектів",</v>
+        <v>"HOURS2":"години",</v>
       </c>
       <c r="J107" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"SOUND_EFF_SET":"Ajustes de efectos de sonido",</v>
+        <v>"HOURS2":"horas",</v>
       </c>
       <c r="K107" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"SOUND_EFF_SET":"Ustawienia efektów dźwiękowych",</v>
+        <v>"HOURS2":"godziny",</v>
       </c>
       <c r="L107" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"SOUND_EFF_SET":"Paramètres des effets sonores",</v>
+        <v>"HOURS2":"heures",</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="15.75" customHeight="1">
       <c r="A108" s="19" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="F108" s="20" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="G108" s="17"/>
       <c r="H108" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"SNAKE":"Snake",</v>
+        <v>"CONTROL_SEVERAL_LAMPS":"Control of several lamps",</v>
       </c>
       <c r="I108" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"SNAKE":"Змійка",</v>
+        <v>"CONTROL_SEVERAL_LAMPS":"Управління кількома лампами",</v>
       </c>
       <c r="J108" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"SNAKE":"Serpiente",</v>
+        <v>"CONTROL_SEVERAL_LAMPS":"Control de varias lámparas",</v>
       </c>
       <c r="K108" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"SNAKE":"Wąż",</v>
+        <v>"CONTROL_SEVERAL_LAMPS":"Sterowanie kilkoma lampami",</v>
       </c>
       <c r="L108" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"SNAKE":"Serpent",</v>
+        <v>"CONTROL_SEVERAL_LAMPS":"Commande de plusieurs lampes",</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="15.75" customHeight="1">
       <c r="A109" s="19" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="F109" s="20" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="G109" s="17"/>
       <c r="H109" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"PARALLEL":"Parallel",</v>
+        <v>"SOUND_EFF_SET":"Sound effects settings",</v>
       </c>
       <c r="I109" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"PARALLEL":"Паралельна",</v>
+        <v>"SOUND_EFF_SET":"Налаштування озвучування ефектів",</v>
       </c>
       <c r="J109" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"PARALLEL":"Paralela",</v>
+        <v>"SOUND_EFF_SET":"Ajustes de efectos de sonido",</v>
       </c>
       <c r="K109" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"PARALLEL":"Równoległy",</v>
+        <v>"SOUND_EFF_SET":"Ustawienia efektów dźwiękowych",</v>
       </c>
       <c r="L109" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"PARALLEL":"Parallèle",</v>
+        <v>"SOUND_EFF_SET":"Paramètres des effets sonores",</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A110" s="25" t="s">
-        <v>612</v>
+      <c r="A110" s="19" t="s">
+        <v>600</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>613</v>
+        <v>601</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
       <c r="F110" s="20" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="G110" s="17"/>
       <c r="H110" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"0_0":"LL corner - to the right",</v>
+        <v>"SNAKE":"Snake",</v>
       </c>
       <c r="I110" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"0_0":"Кут ЛН - вправо",</v>
+        <v>"SNAKE":"Змійка",</v>
       </c>
       <c r="J110" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"0_0":"Esquina LL - a la derecha",</v>
+        <v>"SNAKE":"Serpiente",</v>
       </c>
       <c r="K110" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"0_0":"Narożnik LL - w prawo",</v>
+        <v>"SNAKE":"Wąż",</v>
       </c>
       <c r="L110" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"0_0":"Coin LL - à droite",</v>
+        <v>"SNAKE":"Serpent",</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A111" s="25" t="s">
-        <v>618</v>
+      <c r="A111" s="19" t="s">
+        <v>606</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="D111" s="16" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="F111" s="20" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="G111" s="17"/>
       <c r="H111" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"0_1":"LL corner - up",</v>
+        <v>"PARALLEL":"Parallel",</v>
       </c>
       <c r="I111" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"0_1":"Кут ЛН - вгору",</v>
+        <v>"PARALLEL":"Паралельна",</v>
       </c>
       <c r="J111" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"0_1":"Esquina LL - arriba",</v>
+        <v>"PARALLEL":"Paralela",</v>
       </c>
       <c r="K111" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"0_1":"Narożnik LL - do góry",</v>
+        <v>"PARALLEL":"Równoległy",</v>
       </c>
       <c r="L111" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"0_1":"Coin LL - vers le haut",</v>
+        <v>"PARALLEL":"Parallèle",</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="15.75" customHeight="1">
       <c r="A112" s="25" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="D112" s="16" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
       <c r="F112" s="20" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="G112" s="17"/>
       <c r="H112" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"1_0":"UL corner -  to the right",</v>
+        <v>"0_0":"LL corner - to the right",</v>
       </c>
       <c r="I112" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"1_0":"Кут ЛВ - вправо",</v>
+        <v>"0_0":"Кут ЛН - вправо",</v>
       </c>
       <c r="J112" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"1_0":"Esquina UL - a la derecha",</v>
+        <v>"0_0":"Esquina LL - a la derecha",</v>
       </c>
       <c r="K112" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"1_0":"Narożnik UL - w prawo",</v>
+        <v>"0_0":"Narożnik LL - w prawo",</v>
       </c>
       <c r="L112" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"1_0":"Coin UL - à droite",</v>
+        <v>"0_0":"Coin LL - à droite",</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="15.75" customHeight="1">
       <c r="A113" s="25" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
       <c r="F113" s="20" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="G113" s="17"/>
       <c r="H113" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"1_3":"UL corner - down",</v>
+        <v>"0_1":"LL corner - up",</v>
       </c>
       <c r="I113" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"1_3":"Кут ЛВ - вниз",</v>
+        <v>"0_1":"Кут ЛН - вгору",</v>
       </c>
       <c r="J113" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"1_3":"Esquina UL - abajo",</v>
+        <v>"0_1":"Esquina LL - arriba",</v>
       </c>
       <c r="K113" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"1_3":"Narożnik UL - dół",</v>
+        <v>"0_1":"Narożnik LL - do góry",</v>
       </c>
       <c r="L113" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"1_3":"Coin UL - vers le bas",</v>
+        <v>"0_1":"Coin LL - vers le haut",</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="15.75" customHeight="1">
       <c r="A114" s="25" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>640</v>
+        <v>628</v>
       </c>
       <c r="F114" s="20" t="s">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="G114" s="17"/>
       <c r="H114" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"2_2":"UR corner - to the  left",</v>
+        <v>"1_0":"UL corner -  to the right",</v>
       </c>
       <c r="I114" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"2_2":"Кут ПВ - вліво",</v>
+        <v>"1_0":"Кут ЛВ - вправо",</v>
       </c>
       <c r="J114" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"2_2":"Esquina UR - a la izquierda",</v>
+        <v>"1_0":"Esquina UL - a la derecha",</v>
       </c>
       <c r="K114" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"2_2":"Narożnik UR - w lewo",</v>
+        <v>"1_0":"Narożnik UL - w prawo",</v>
       </c>
       <c r="L114" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"2_2":"Coin UR - à gauche",</v>
+        <v>"1_0":"Coin UL - à droite",</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="15.75" customHeight="1">
       <c r="A115" s="25" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>643</v>
+        <v>631</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
       <c r="F115" s="20" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
       <c r="G115" s="17"/>
       <c r="H115" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"2_3":"UR corner - down",</v>
+        <v>"1_3":"UL corner - down",</v>
       </c>
       <c r="I115" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"2_3":"Кут ПВ - вниз",</v>
+        <v>"1_3":"Кут ЛВ - вниз",</v>
       </c>
       <c r="J115" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"2_3":"Esquina UR - abajo",</v>
+        <v>"1_3":"Esquina UL - abajo",</v>
       </c>
       <c r="K115" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"2_3":"Narożnik UR - dół",</v>
+        <v>"1_3":"Narożnik UL - dół",</v>
       </c>
       <c r="L115" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"2_3":"Coin UR - vers le bas",</v>
+        <v>"1_3":"Coin UL - vers le bas",</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="15.75" customHeight="1">
       <c r="A116" s="25" t="s">
-        <v>648</v>
+        <v>636</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>649</v>
+        <v>637</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>650</v>
+        <v>638</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>651</v>
+        <v>639</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>652</v>
+        <v>640</v>
       </c>
       <c r="F116" s="20" t="s">
-        <v>653</v>
+        <v>641</v>
       </c>
       <c r="G116" s="17"/>
       <c r="H116" s="19" t="str">
         <f t="shared" si="30"/>
-        <v>"3_2":"LR corner - to the  left",</v>
+        <v>"2_2":"UR corner - to the  left",</v>
       </c>
       <c r="I116" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>"3_2":"Кут ПН - вліво",</v>
+        <v>"2_2":"Кут ПВ - вліво",</v>
       </c>
       <c r="J116" s="19" t="str">
         <f t="shared" si="32"/>
-        <v>"3_2":"Esquina LR - a la izquierda",</v>
+        <v>"2_2":"Esquina UR - a la izquierda",</v>
       </c>
       <c r="K116" s="19" t="str">
         <f t="shared" si="33"/>
-        <v>"3_2":"Narożnik LR - w lewo",</v>
+        <v>"2_2":"Narożnik UR - w lewo",</v>
       </c>
       <c r="L116" s="22" t="str">
         <f t="shared" si="34"/>
-        <v>"3_2":"Coin LR - à gauche",</v>
+        <v>"2_2":"Coin UR - à gauche",</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="15.75" customHeight="1">
       <c r="A117" s="25" t="s">
-        <v>654</v>
+        <v>642</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>655</v>
+        <v>643</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
       <c r="D117" s="16" t="s">
-        <v>657</v>
+        <v>645</v>
       </c>
       <c r="E117" s="16" t="s">
-        <v>658</v>
+        <v>646</v>
       </c>
       <c r="F117" s="20" t="s">
-        <v>659</v>
+        <v>647</v>
       </c>
       <c r="G117" s="17"/>
       <c r="H117" s="19" t="str">
-        <f>CONCATENATE("""",A117,"""",":","""",B117,"""")</f>
+        <f t="shared" si="30"/>
+        <v>"2_3":"UR corner - down",</v>
+      </c>
+      <c r="I117" s="21" t="str">
+        <f t="shared" si="31"/>
+        <v>"2_3":"Кут ПВ - вниз",</v>
+      </c>
+      <c r="J117" s="19" t="str">
+        <f t="shared" si="32"/>
+        <v>"2_3":"Esquina UR - abajo",</v>
+      </c>
+      <c r="K117" s="19" t="str">
+        <f t="shared" si="33"/>
+        <v>"2_3":"Narożnik UR - dół",</v>
+      </c>
+      <c r="L117" s="22" t="str">
+        <f t="shared" si="34"/>
+        <v>"2_3":"Coin UR - vers le bas",</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A118" s="25" t="s">
+        <v>648</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>649</v>
+      </c>
+      <c r="C118" s="19" t="s">
+        <v>650</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>651</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>652</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="G118" s="17"/>
+      <c r="H118" s="19" t="str">
+        <f t="shared" si="30"/>
+        <v>"3_2":"LR corner - to the  left",</v>
+      </c>
+      <c r="I118" s="21" t="str">
+        <f t="shared" si="31"/>
+        <v>"3_2":"Кут ПН - вліво",</v>
+      </c>
+      <c r="J118" s="19" t="str">
+        <f t="shared" si="32"/>
+        <v>"3_2":"Esquina LR - a la izquierda",</v>
+      </c>
+      <c r="K118" s="19" t="str">
+        <f t="shared" si="33"/>
+        <v>"3_2":"Narożnik LR - w lewo",</v>
+      </c>
+      <c r="L118" s="22" t="str">
+        <f t="shared" si="34"/>
+        <v>"3_2":"Coin LR - à gauche",</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A119" s="25" t="s">
+        <v>654</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>655</v>
+      </c>
+      <c r="C119" s="19" t="s">
+        <v>656</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>657</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>658</v>
+      </c>
+      <c r="F119" s="20" t="s">
+        <v>659</v>
+      </c>
+      <c r="G119" s="17"/>
+      <c r="H119" s="19" t="str">
+        <f>CONCATENATE("""",A119,"""",":","""",B119,"""")</f>
         <v>"3_1":"LR corner - up"</v>
       </c>
-      <c r="I117" s="21" t="str">
-        <f>CONCATENATE("""",A117,"""",":","""",C117,"""")</f>
+      <c r="I119" s="21" t="str">
+        <f>CONCATENATE("""",A119,"""",":","""",C119,"""")</f>
         <v>"3_1":"Кут ПН - вгору"</v>
       </c>
-      <c r="J117" s="19" t="str">
-        <f>CONCATENATE("""",A117,"""",":","""",D117,"""")</f>
+      <c r="J119" s="19" t="str">
+        <f>CONCATENATE("""",A119,"""",":","""",D119,"""")</f>
         <v>"3_1":"Esquina LR - arriba"</v>
       </c>
-      <c r="K117" s="19" t="str">
-        <f>CONCATENATE("""",A117,"""",":","""",E117,"""")</f>
+      <c r="K119" s="19" t="str">
+        <f>CONCATENATE("""",A119,"""",":","""",E119,"""")</f>
         <v>"3_1":"Narożnik LR - do góry"</v>
       </c>
-      <c r="L117" s="22" t="str">
-        <f>CONCATENATE("""",A117,"""",":","""",F117,"""")</f>
+      <c r="L119" s="22" t="str">
+        <f>CONCATENATE("""",A119,"""",":","""",F119,"""")</f>
         <v>"3_1":"Coin LR - vers le haut"</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A118" s="19" t="s">
+    <row r="120" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A120" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="16"/>
-      <c r="E118" s="16"/>
-      <c r="F118" s="16"/>
-      <c r="G118" s="17"/>
-      <c r="H118" s="19" t="s">
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="19" t="s">
         <v>660</v>
       </c>
-      <c r="I118" s="21" t="s">
+      <c r="I120" s="21" t="s">
         <v>660</v>
       </c>
-      <c r="J118" s="19" t="s">
+      <c r="J120" s="19" t="s">
         <v>660</v>
       </c>
-      <c r="K118" s="21" t="s">
+      <c r="K120" s="21" t="s">
         <v>660</v>
       </c>
-      <c r="L118" s="26" t="s">
+      <c r="L120" s="26" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="15.75" customHeight="1">
-      <c r="G119" s="27"/>
-    </row>
-    <row r="120" spans="1:12" ht="15.75" customHeight="1">
-      <c r="J120" s="16"/>
-    </row>
-    <row r="121" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="122" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="121" spans="1:12" ht="15.75" customHeight="1">
+      <c r="G121" s="27"/>
+    </row>
+    <row r="122" spans="1:12" ht="15.75" customHeight="1">
+      <c r="J122" s="16"/>
+    </row>
     <row r="123" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="124" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="125" spans="1:12" ht="15.75" customHeight="1"/>
@@ -7110,12 +7226,8 @@
     <row r="148" spans="11:11" ht="15.75" customHeight="1"/>
     <row r="149" spans="11:11" ht="15.75" customHeight="1"/>
     <row r="150" spans="11:11" ht="15.75" customHeight="1"/>
-    <row r="151" spans="11:11" ht="15.75" customHeight="1">
-      <c r="K151" s="21"/>
-    </row>
-    <row r="152" spans="11:11" ht="15.75" customHeight="1">
-      <c r="K152" s="21"/>
-    </row>
+    <row r="151" spans="11:11" ht="15.75" customHeight="1"/>
+    <row r="152" spans="11:11" ht="15.75" customHeight="1"/>
     <row r="153" spans="11:11" ht="15.75" customHeight="1">
       <c r="K153" s="21"/>
     </row>
@@ -7158,8 +7270,12 @@
     <row r="166" spans="11:11" ht="15.75" customHeight="1">
       <c r="K166" s="21"/>
     </row>
-    <row r="167" spans="11:11" ht="15.75" customHeight="1"/>
-    <row r="168" spans="11:11" ht="15.75" customHeight="1"/>
+    <row r="167" spans="11:11" ht="15.75" customHeight="1">
+      <c r="K167" s="21"/>
+    </row>
+    <row r="168" spans="11:11" ht="15.75" customHeight="1">
+      <c r="K168" s="21"/>
+    </row>
     <row r="169" spans="11:11" ht="15.75" customHeight="1"/>
     <row r="170" spans="11:11" ht="15.75" customHeight="1"/>
     <row r="171" spans="11:11" ht="15.75" customHeight="1"/>
@@ -7991,18 +8107,11 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:M150"/>
+  <autoFilter ref="A1:M152"/>
   <customSheetViews>
-    <customSheetView guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K150"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="67239803"/>
-        </ext>
-      </extLst>
-    </customSheetView>
     <customSheetView guid="{02F08554-2E03-4827-AA05-82E0997FBBA8}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:K150">
@@ -8124,6 +8233,15 @@
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="300842063"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:K150"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="67239803"/>
         </ext>
       </extLst>
     </customSheetView>

</xml_diff>

<commit_message>
Correct Lamp turn off. (Seved files damage)
Змінена послідовність вимикання лампи (Була можливість пошкодження файлив ,що  зберігаються)
</commit_message>
<xml_diff>
--- a/FieryLedLampMultilingual/Language.xlsx
+++ b/FieryLedLampMultilingual/Language.xlsx
@@ -18,8 +18,8 @@
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
+    <customWorkbookView name="Фильтр 2" guid="{02F08554-2E03-4827-AA05-82E0997FBBA8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Фильтр 1" guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Фильтр 2" guid="{02F08554-2E03-4827-AA05-82E0997FBBA8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -251,9 +251,6 @@
     <t>S_VOLUM</t>
   </si>
   <si>
-    <t>Sound Volum</t>
-  </si>
-  <si>
     <t>Гучність</t>
   </si>
   <si>
@@ -2052,6 +2049,9 @@
   </si>
   <si>
     <t>Hardware Setings</t>
+  </si>
+  <si>
+    <t>Sound Volume</t>
   </si>
 </sst>
 </file>
@@ -2435,9 +2435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2964,24 +2964,24 @@
         <v>72</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>77</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="19" t="str">
         <f t="shared" si="0"/>
-        <v>"S_VOLUM":"Sound Volum",</v>
+        <v>"S_VOLUM":"Sound Volume",</v>
       </c>
       <c r="I13" s="21" t="str">
         <f t="shared" si="1"/>
@@ -3002,22 +3002,22 @@
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="C14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>83</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="19" t="str">
@@ -3043,22 +3043,22 @@
     </row>
     <row r="15" spans="1:28">
       <c r="A15" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>89</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="19" t="str">
@@ -3095,22 +3095,22 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="F17" s="20" t="s">
         <v>94</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>95</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="19" t="str">
@@ -3136,22 +3136,22 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="E18" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>101</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="19" t="str">
@@ -3177,22 +3177,22 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="19" t="str">
@@ -3229,22 +3229,22 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="F21" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>113</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="19" t="str">
@@ -3270,22 +3270,22 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="E22" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="F22" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>119</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="19" t="str">
@@ -3311,22 +3311,22 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="F23" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>125</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="19" t="str">
@@ -3352,22 +3352,22 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="E24" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="F24" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="19" t="str">
@@ -3393,22 +3393,22 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="E25" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="F25" s="20" t="s">
         <v>136</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>137</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="19" t="str">
@@ -3434,22 +3434,22 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="E26" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="F26" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>143</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="19" t="str">
@@ -3475,22 +3475,22 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="D27" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>149</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="19" t="str">
@@ -3516,22 +3516,22 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="C28" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="E28" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="F28" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>155</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="19" t="str">
@@ -3557,22 +3557,22 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="F29" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>161</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="19" t="str">
@@ -3598,22 +3598,22 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="E30" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="F30" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>167</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="19" t="str">
@@ -3639,22 +3639,22 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="D31" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="E31" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="F31" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="19" t="str">
@@ -3680,22 +3680,22 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="F32" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>179</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="19" t="str">
@@ -3721,22 +3721,22 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="E33" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="F33" s="20" t="s">
         <v>184</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>185</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="19" t="str">
@@ -3762,22 +3762,22 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="E34" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="F34" s="20" t="s">
         <v>190</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>191</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="19" t="str">
@@ -3803,22 +3803,22 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="E35" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="F35" s="20" t="s">
         <v>196</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>197</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="19" t="str">
@@ -3844,22 +3844,22 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="C36" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="D36" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="E36" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="F36" s="20" t="s">
         <v>202</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>203</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="19" t="str">
@@ -3885,22 +3885,22 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="C37" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="D37" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="E37" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="F37" s="20" t="s">
         <v>208</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>209</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="19" t="str">
@@ -3926,22 +3926,22 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="C38" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="D38" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="E38" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>214</v>
-      </c>
       <c r="F38" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G38" s="17"/>
       <c r="H38" s="19" t="str">
@@ -3978,22 +3978,22 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="C40" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="D40" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="E40" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="F40" s="20" t="s">
         <v>219</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>220</v>
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="19" t="str">
@@ -4019,22 +4019,22 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C41" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="D41" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="E41" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="F41" s="20" t="s">
         <v>225</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>226</v>
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="19" t="str">
@@ -4060,22 +4060,22 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="C42" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="D42" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="F42" s="20" t="s">
         <v>231</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>232</v>
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="19" t="str">
@@ -4101,22 +4101,22 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="C43" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="D43" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="E43" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="F43" s="20" t="s">
         <v>237</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="19" t="str">
@@ -4153,22 +4153,22 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="C45" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E45" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="F45" s="20" t="s">
         <v>243</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>244</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="19" t="str">
@@ -4194,22 +4194,22 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="E46" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="F46" s="20" t="s">
         <v>249</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>250</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="19" t="str">
@@ -4235,22 +4235,22 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="C47" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="D47" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="F47" s="20" t="s">
         <v>255</v>
-      </c>
-      <c r="F47" s="20" t="s">
-        <v>256</v>
       </c>
       <c r="G47" s="17"/>
       <c r="H47" s="19" t="str">
@@ -4276,22 +4276,22 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="C48" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="E48" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="20" t="s">
         <v>261</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>262</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="19" t="str">
@@ -4328,30 +4328,30 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B50" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="C50" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="D50" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="E50" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="F50" s="20" t="s">
         <v>267</v>
-      </c>
-      <c r="F50" s="20" t="s">
-        <v>268</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="19" t="str">
-        <f t="shared" ref="H50:H75" si="25">CONCATENATE("""",A50,"""",":","""",B50,"""",",")</f>
+        <f t="shared" ref="H50:H74" si="25">CONCATENATE("""",A50,"""",":","""",B50,"""",",")</f>
         <v>"USE_PASS":"Use a password to access this page",</v>
       </c>
       <c r="I50" s="21" t="str">
-        <f t="shared" ref="I50:I75" si="26">CONCATENATE("""",A50,"""",":","""",C50,"""",",")</f>
+        <f t="shared" ref="I50:I74" si="26">CONCATENATE("""",A50,"""",":","""",C50,"""",",")</f>
         <v>"USE_PASS":"Використовувати пароль для доступу до цієї сторінки",</v>
       </c>
       <c r="J50" s="19" t="str">
@@ -4369,22 +4369,22 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="C51" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="D51" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="E51" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="F51" s="20" t="s">
         <v>273</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>274</v>
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="19" t="str">
@@ -4410,22 +4410,22 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="D52" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="E52" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="F52" s="20" t="s">
         <v>279</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>280</v>
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="19" t="str">
@@ -4451,22 +4451,22 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="C53" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="D53" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="E53" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="F53" s="20" t="s">
         <v>285</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>286</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="19" t="str">
@@ -4492,22 +4492,22 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="D54" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="E54" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="F54" s="20" t="s">
         <v>291</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>292</v>
       </c>
       <c r="G54" s="17"/>
       <c r="H54" s="19" t="str">
@@ -4533,22 +4533,22 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="C55" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="D55" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="E55" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="F55" s="20" t="s">
         <v>297</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>298</v>
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="19" t="str">
@@ -4574,22 +4574,22 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="C56" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="D56" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="E56" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="F56" s="20" t="s">
         <v>303</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>304</v>
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="19" t="str">
@@ -4615,22 +4615,22 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="C57" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="D57" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="E57" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="F57" s="20" t="s">
         <v>309</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>310</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="19" t="str">
@@ -4656,22 +4656,22 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="C58" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="D58" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="E58" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="F58" s="20" t="s">
         <v>315</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>316</v>
       </c>
       <c r="G58" s="17"/>
       <c r="H58" s="19" t="str">
@@ -4697,22 +4697,22 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="C59" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="D59" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="E59" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="F59" s="20" t="s">
         <v>321</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>322</v>
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="19" t="str">
@@ -4738,22 +4738,22 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="C60" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="D60" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="E60" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="F60" s="20" t="s">
         <v>327</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>328</v>
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="19" t="str">
@@ -4779,22 +4779,22 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="B61" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="C61" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="D61" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="E61" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="F61" s="20" t="s">
         <v>333</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>334</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="19" t="str">
@@ -4820,22 +4820,22 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B62" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="C62" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="D62" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="E62" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="F62" s="20" t="s">
         <v>339</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>340</v>
       </c>
       <c r="G62" s="17"/>
       <c r="H62" s="19" t="str">
@@ -4861,22 +4861,22 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B63" s="19" t="s">
         <v>341</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="C63" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="D63" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="E63" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="F63" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>346</v>
       </c>
       <c r="G63" s="17"/>
       <c r="H63" s="19" t="str">
@@ -4902,22 +4902,22 @@
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B64" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="C64" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="D64" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="E64" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="F64" s="20" t="s">
         <v>351</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>352</v>
       </c>
       <c r="G64" s="17"/>
       <c r="H64" s="19" t="str">
@@ -4943,22 +4943,22 @@
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="B65" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="C65" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="D65" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="E65" s="16" t="s">
         <v>356</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="F65" s="20" t="s">
         <v>357</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>358</v>
       </c>
       <c r="G65" s="17"/>
       <c r="H65" s="19" t="str">
@@ -4984,22 +4984,22 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B66" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="C66" s="19" t="s">
         <v>360</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="D66" s="16" t="s">
         <v>361</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="E66" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="F66" s="20" t="s">
         <v>363</v>
-      </c>
-      <c r="F66" s="20" t="s">
-        <v>364</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="19" t="str">
@@ -5025,22 +5025,22 @@
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1">
       <c r="A67" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="B67" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="C67" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="D67" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="E67" s="16" t="s">
         <v>368</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="F67" s="20" t="s">
         <v>369</v>
-      </c>
-      <c r="F67" s="20" t="s">
-        <v>370</v>
       </c>
       <c r="G67" s="17"/>
       <c r="H67" s="19" t="str">
@@ -5066,22 +5066,22 @@
     </row>
     <row r="68" spans="1:12" ht="15.75" customHeight="1">
       <c r="A68" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="C68" s="19" t="s">
         <v>372</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="D68" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="E68" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="F68" s="20" t="s">
         <v>375</v>
-      </c>
-      <c r="F68" s="20" t="s">
-        <v>376</v>
       </c>
       <c r="G68" s="17"/>
       <c r="H68" s="19" t="str">
@@ -5107,22 +5107,22 @@
     </row>
     <row r="69" spans="1:12" ht="15.75" customHeight="1">
       <c r="A69" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B69" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="C69" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="D69" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="E69" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="F69" s="20" t="s">
         <v>381</v>
-      </c>
-      <c r="F69" s="20" t="s">
-        <v>382</v>
       </c>
       <c r="G69" s="17"/>
       <c r="H69" s="19" t="str">
@@ -5148,22 +5148,22 @@
     </row>
     <row r="70" spans="1:12" ht="15.75" customHeight="1">
       <c r="A70" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>383</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="C70" s="19" t="s">
         <v>384</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="D70" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="E70" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="F70" s="20" t="s">
         <v>387</v>
-      </c>
-      <c r="F70" s="20" t="s">
-        <v>388</v>
       </c>
       <c r="G70" s="17"/>
       <c r="H70" s="19" t="str">
@@ -5189,22 +5189,22 @@
     </row>
     <row r="71" spans="1:12" ht="15.75" customHeight="1">
       <c r="A71" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="C71" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="D71" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="E71" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="F71" s="20" t="s">
         <v>393</v>
-      </c>
-      <c r="F71" s="20" t="s">
-        <v>394</v>
       </c>
       <c r="G71" s="17"/>
       <c r="H71" s="19" t="str">
@@ -5230,22 +5230,22 @@
     </row>
     <row r="72" spans="1:12" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="19" t="s">
+        <v>667</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>672</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>671</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>669</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="F72" s="22" t="s">
         <v>668</v>
-      </c>
-      <c r="B72" s="19" t="s">
-        <v>673</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>672</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>670</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>671</v>
-      </c>
-      <c r="F72" s="22" t="s">
-        <v>669</v>
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="19" t="str">
@@ -5271,22 +5271,22 @@
     </row>
     <row r="73" spans="1:12" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>665</v>
+      </c>
+      <c r="E73" s="23" t="s">
         <v>664</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>663</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>662</v>
-      </c>
-      <c r="D73" s="23" t="s">
+      <c r="F73" s="23" t="s">
         <v>666</v>
-      </c>
-      <c r="E73" s="23" t="s">
-        <v>665</v>
-      </c>
-      <c r="F73" s="23" t="s">
-        <v>667</v>
       </c>
       <c r="G73" s="17"/>
       <c r="H73" s="19" t="str">
@@ -5312,22 +5312,22 @@
     </row>
     <row r="74" spans="1:12" ht="15.75" customHeight="1">
       <c r="A74" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="B74" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="C74" s="19" t="s">
+        <v>660</v>
+      </c>
+      <c r="D74" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="C74" s="19" t="s">
-        <v>661</v>
-      </c>
-      <c r="D74" s="16" t="s">
+      <c r="E74" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="F74" s="20" t="s">
         <v>398</v>
-      </c>
-      <c r="F74" s="20" t="s">
-        <v>399</v>
       </c>
       <c r="G74" s="17"/>
       <c r="H74" s="19" t="str">
@@ -5364,22 +5364,22 @@
     </row>
     <row r="76" spans="1:12" ht="15.75" customHeight="1">
       <c r="A76" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="C76" s="19" t="s">
         <v>401</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="D76" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="E76" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="F76" s="20" t="s">
         <v>404</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>405</v>
       </c>
       <c r="G76" s="17"/>
       <c r="H76" s="19" t="str">
@@ -5405,22 +5405,22 @@
     </row>
     <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="C77" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="D77" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="E77" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="F77" s="20" t="s">
         <v>410</v>
-      </c>
-      <c r="F77" s="20" t="s">
-        <v>411</v>
       </c>
       <c r="G77" s="17"/>
       <c r="H77" s="19" t="str">
@@ -5446,22 +5446,22 @@
     </row>
     <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="C78" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="D78" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="E78" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="F78" s="20" t="s">
         <v>416</v>
-      </c>
-      <c r="F78" s="20" t="s">
-        <v>417</v>
       </c>
       <c r="G78" s="17"/>
       <c r="H78" s="19" t="str">
@@ -5487,22 +5487,22 @@
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="C79" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="D79" s="16" t="s">
         <v>420</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="E79" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="F79" s="20" t="s">
         <v>422</v>
-      </c>
-      <c r="F79" s="20" t="s">
-        <v>423</v>
       </c>
       <c r="G79" s="17"/>
       <c r="H79" s="19" t="str">
@@ -5528,22 +5528,22 @@
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="B80" s="19" t="s">
+      <c r="C80" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="D80" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="D80" s="23" t="s">
+      <c r="E80" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="E80" s="24" t="s">
+      <c r="F80" s="23" t="s">
         <v>428</v>
-      </c>
-      <c r="F80" s="23" t="s">
-        <v>429</v>
       </c>
       <c r="G80" s="17"/>
       <c r="H80" s="19" t="str">
@@ -5569,22 +5569,22 @@
     </row>
     <row r="81" spans="1:12" ht="15.75" customHeight="1">
       <c r="A81" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="B81" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="B81" s="19" t="s">
+      <c r="C81" s="19" t="s">
         <v>431</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="D81" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="E81" s="16" t="s">
         <v>433</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="F81" s="19" t="s">
         <v>434</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>435</v>
       </c>
       <c r="G81" s="17"/>
       <c r="H81" s="19" t="str">
@@ -5610,22 +5610,22 @@
     </row>
     <row r="82" spans="1:12" ht="15.75" customHeight="1">
       <c r="A82" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>436</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="C82" s="19" t="s">
         <v>437</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="D82" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="D82" s="16" t="s">
+      <c r="E82" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="F82" s="20" t="s">
         <v>440</v>
-      </c>
-      <c r="F82" s="20" t="s">
-        <v>441</v>
       </c>
       <c r="G82" s="17"/>
       <c r="H82" s="19" t="str">
@@ -5651,22 +5651,22 @@
     </row>
     <row r="83" spans="1:12" ht="15.75" customHeight="1">
       <c r="A83" s="19" t="s">
+        <v>441</v>
+      </c>
+      <c r="B83" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="C83" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="D83" s="16" t="s">
         <v>444</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="E83" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="F83" s="20" t="s">
         <v>446</v>
-      </c>
-      <c r="F83" s="20" t="s">
-        <v>447</v>
       </c>
       <c r="G83" s="17"/>
       <c r="H83" s="19" t="str">
@@ -5692,22 +5692,22 @@
     </row>
     <row r="84" spans="1:12" ht="15.75" customHeight="1">
       <c r="A84" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="B84" s="19" t="s">
         <v>448</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="C84" s="19" t="s">
         <v>449</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="D84" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="E84" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="F84" s="20" t="s">
         <v>452</v>
-      </c>
-      <c r="F84" s="20" t="s">
-        <v>453</v>
       </c>
       <c r="G84" s="17"/>
       <c r="H84" s="19" t="str">
@@ -5733,22 +5733,22 @@
     </row>
     <row r="85" spans="1:12" ht="15.75" customHeight="1">
       <c r="A85" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B85" s="19" t="s">
         <v>454</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="C85" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="D85" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="E85" s="16" t="s">
         <v>457</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="F85" s="20" t="s">
         <v>458</v>
-      </c>
-      <c r="F85" s="20" t="s">
-        <v>459</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="19" t="str">
@@ -5774,22 +5774,22 @@
     </row>
     <row r="86" spans="1:12" ht="15.75" customHeight="1">
       <c r="A86" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="B86" s="19" t="s">
         <v>460</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="C86" s="19" t="s">
         <v>461</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="D86" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="E86" s="16" t="s">
         <v>463</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="F86" s="20" t="s">
         <v>464</v>
-      </c>
-      <c r="F86" s="20" t="s">
-        <v>465</v>
       </c>
       <c r="G86" s="17"/>
       <c r="H86" s="19" t="str">
@@ -5815,22 +5815,22 @@
     </row>
     <row r="87" spans="1:12" ht="15.75" customHeight="1">
       <c r="A87" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="C87" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="D87" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="E87" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="F87" s="20" t="s">
         <v>470</v>
-      </c>
-      <c r="F87" s="20" t="s">
-        <v>471</v>
       </c>
       <c r="G87" s="17"/>
       <c r="H87" s="19" t="str">
@@ -5856,22 +5856,22 @@
     </row>
     <row r="88" spans="1:12" ht="15.75" customHeight="1">
       <c r="A88" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="C88" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="D88" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="E88" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="F88" s="20" t="s">
         <v>476</v>
-      </c>
-      <c r="F88" s="20" t="s">
-        <v>477</v>
       </c>
       <c r="G88" s="17"/>
       <c r="H88" s="19" t="str">
@@ -5897,22 +5897,22 @@
     </row>
     <row r="89" spans="1:12" ht="15.75" customHeight="1">
       <c r="A89" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="B89" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="C89" s="19" t="s">
         <v>479</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="D89" s="16" t="s">
         <v>480</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="E89" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="F89" s="20" t="s">
         <v>482</v>
-      </c>
-      <c r="F89" s="20" t="s">
-        <v>483</v>
       </c>
       <c r="G89" s="17"/>
       <c r="H89" s="19" t="str">
@@ -5938,22 +5938,22 @@
     </row>
     <row r="90" spans="1:12" ht="15.75" customHeight="1">
       <c r="A90" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="B90" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="B90" s="19" t="s">
+      <c r="C90" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="D90" s="16" t="s">
         <v>486</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="E90" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="F90" s="20" t="s">
         <v>488</v>
-      </c>
-      <c r="F90" s="20" t="s">
-        <v>489</v>
       </c>
       <c r="G90" s="17"/>
       <c r="H90" s="19" t="str">
@@ -5979,22 +5979,22 @@
     </row>
     <row r="91" spans="1:12" ht="15.75" customHeight="1">
       <c r="A91" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>490</v>
       </c>
-      <c r="B91" s="19" t="s">
+      <c r="C91" s="19" t="s">
         <v>491</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="D91" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="E91" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="F91" s="20" t="s">
         <v>494</v>
-      </c>
-      <c r="F91" s="20" t="s">
-        <v>495</v>
       </c>
       <c r="G91" s="17"/>
       <c r="H91" s="19" t="str">
@@ -6020,22 +6020,22 @@
     </row>
     <row r="92" spans="1:12" ht="15.75" customHeight="1">
       <c r="A92" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>496</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="C92" s="19" t="s">
         <v>497</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="D92" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="E92" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="F92" s="20" t="s">
         <v>500</v>
-      </c>
-      <c r="F92" s="20" t="s">
-        <v>501</v>
       </c>
       <c r="G92" s="17"/>
       <c r="H92" s="19" t="str">
@@ -6061,22 +6061,22 @@
     </row>
     <row r="93" spans="1:12" ht="15.75" customHeight="1">
       <c r="A93" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>502</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="C93" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="D93" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="E93" s="16" t="s">
         <v>505</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="F93" s="20" t="s">
         <v>506</v>
-      </c>
-      <c r="F93" s="20" t="s">
-        <v>507</v>
       </c>
       <c r="G93" s="17"/>
       <c r="H93" s="19" t="str">
@@ -6102,22 +6102,22 @@
     </row>
     <row r="94" spans="1:12" ht="15.75" customHeight="1">
       <c r="A94" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="B94" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="C94" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="D94" s="16" t="s">
         <v>510</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="E94" s="16" t="s">
         <v>511</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="F94" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="F94" s="20" t="s">
-        <v>513</v>
       </c>
       <c r="G94" s="17"/>
       <c r="H94" s="19" t="str">
@@ -6143,22 +6143,22 @@
     </row>
     <row r="95" spans="1:12" ht="15.75" customHeight="1">
       <c r="A95" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="B95" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="C95" s="19" t="s">
         <v>515</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="D95" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="D95" s="16" t="s">
+      <c r="E95" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="F95" s="20" t="s">
         <v>518</v>
-      </c>
-      <c r="F95" s="20" t="s">
-        <v>519</v>
       </c>
       <c r="G95" s="17"/>
       <c r="H95" s="19" t="str">
@@ -6184,22 +6184,22 @@
     </row>
     <row r="96" spans="1:12" ht="15.75" customHeight="1">
       <c r="A96" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="B96" s="19" t="s">
         <v>520</v>
       </c>
-      <c r="B96" s="19" t="s">
+      <c r="C96" s="19" t="s">
         <v>521</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="D96" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="D96" s="16" t="s">
+      <c r="E96" s="16" t="s">
         <v>523</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="F96" s="20" t="s">
         <v>524</v>
-      </c>
-      <c r="F96" s="20" t="s">
-        <v>525</v>
       </c>
       <c r="G96" s="17"/>
       <c r="H96" s="19" t="str">
@@ -6225,22 +6225,22 @@
     </row>
     <row r="97" spans="1:12" ht="15.75" customHeight="1">
       <c r="A97" s="19" t="s">
+        <v>525</v>
+      </c>
+      <c r="B97" s="19" t="s">
         <v>526</v>
       </c>
-      <c r="B97" s="19" t="s">
+      <c r="C97" s="19" t="s">
         <v>527</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="D97" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="E97" s="16" t="s">
         <v>529</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="F97" s="20" t="s">
         <v>530</v>
-      </c>
-      <c r="F97" s="20" t="s">
-        <v>531</v>
       </c>
       <c r="G97" s="17"/>
       <c r="H97" s="19" t="str">
@@ -6266,22 +6266,22 @@
     </row>
     <row r="98" spans="1:12" ht="15.75" customHeight="1">
       <c r="A98" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="B98" s="19" t="s">
         <v>532</v>
       </c>
-      <c r="B98" s="19" t="s">
+      <c r="C98" s="19" t="s">
         <v>533</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="D98" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="D98" s="16" t="s">
+      <c r="E98" s="16" t="s">
         <v>535</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="20" t="s">
         <v>536</v>
-      </c>
-      <c r="F98" s="20" t="s">
-        <v>537</v>
       </c>
       <c r="G98" s="17"/>
       <c r="H98" s="19" t="str">
@@ -6307,22 +6307,22 @@
     </row>
     <row r="99" spans="1:12" ht="15.75" customHeight="1">
       <c r="A99" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="B99" s="19" t="s">
         <v>538</v>
       </c>
-      <c r="B99" s="19" t="s">
+      <c r="C99" s="19" t="s">
         <v>539</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="D99" s="20" t="s">
         <v>540</v>
       </c>
-      <c r="D99" s="20" t="s">
+      <c r="E99" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="E99" s="20" t="s">
+      <c r="F99" s="20" t="s">
         <v>542</v>
-      </c>
-      <c r="F99" s="20" t="s">
-        <v>543</v>
       </c>
       <c r="G99" s="17"/>
       <c r="H99" s="19" t="str">
@@ -6348,22 +6348,22 @@
     </row>
     <row r="100" spans="1:12" ht="15.75" customHeight="1">
       <c r="A100" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="B100" s="19" t="s">
         <v>544</v>
       </c>
-      <c r="B100" s="19" t="s">
+      <c r="C100" s="19" t="s">
         <v>545</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="D100" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="D100" s="16" t="s">
+      <c r="E100" s="16" t="s">
         <v>547</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="F100" s="20" t="s">
         <v>548</v>
-      </c>
-      <c r="F100" s="20" t="s">
-        <v>549</v>
       </c>
       <c r="G100" s="17"/>
       <c r="H100" s="19" t="str">
@@ -6389,22 +6389,22 @@
     </row>
     <row r="101" spans="1:12" ht="15.75" customHeight="1">
       <c r="A101" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>550</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="C101" s="19" t="s">
         <v>551</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="D101" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="D101" s="16" t="s">
+      <c r="E101" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="F101" s="20" t="s">
         <v>554</v>
-      </c>
-      <c r="F101" s="20" t="s">
-        <v>555</v>
       </c>
       <c r="G101" s="17"/>
       <c r="H101" s="19" t="str">
@@ -6430,22 +6430,22 @@
     </row>
     <row r="102" spans="1:12" ht="15.75" customHeight="1">
       <c r="A102" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="B102" s="19" t="s">
         <v>556</v>
       </c>
-      <c r="B102" s="19" t="s">
+      <c r="C102" s="19" t="s">
         <v>557</v>
       </c>
-      <c r="C102" s="19" t="s">
+      <c r="D102" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="D102" s="16" t="s">
+      <c r="E102" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="F102" s="20" t="s">
         <v>560</v>
-      </c>
-      <c r="F102" s="20" t="s">
-        <v>561</v>
       </c>
       <c r="G102" s="17"/>
       <c r="H102" s="19" t="str">
@@ -6471,22 +6471,22 @@
     </row>
     <row r="103" spans="1:12" ht="15.75" customHeight="1">
       <c r="A103" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="B103" s="19" t="s">
         <v>562</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="C103" s="19" t="s">
         <v>563</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="D103" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="D103" s="16" t="s">
+      <c r="E103" s="16" t="s">
         <v>565</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="F103" s="20" t="s">
         <v>566</v>
-      </c>
-      <c r="F103" s="20" t="s">
-        <v>567</v>
       </c>
       <c r="G103" s="17"/>
       <c r="H103" s="19" t="str">
@@ -6512,22 +6512,22 @@
     </row>
     <row r="104" spans="1:12" ht="15.75" customHeight="1">
       <c r="A104" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>568</v>
       </c>
-      <c r="B104" s="19" t="s">
+      <c r="C104" s="19" t="s">
         <v>569</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="D104" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="E104" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="F104" s="20" t="s">
         <v>572</v>
-      </c>
-      <c r="F104" s="20" t="s">
-        <v>573</v>
       </c>
       <c r="G104" s="17"/>
       <c r="H104" s="19" t="str">
@@ -6553,22 +6553,22 @@
     </row>
     <row r="105" spans="1:12" ht="15.75" customHeight="1">
       <c r="A105" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>574</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="C105" s="19" t="s">
         <v>575</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="D105" s="16" t="s">
         <v>576</v>
       </c>
-      <c r="D105" s="16" t="s">
+      <c r="E105" s="16" t="s">
         <v>577</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="F105" s="20" t="s">
         <v>578</v>
-      </c>
-      <c r="F105" s="20" t="s">
-        <v>579</v>
       </c>
       <c r="G105" s="17"/>
       <c r="H105" s="19" t="str">
@@ -6594,22 +6594,22 @@
     </row>
     <row r="106" spans="1:12" ht="15.75" customHeight="1">
       <c r="A106" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>580</v>
       </c>
-      <c r="B106" s="19" t="s">
+      <c r="C106" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="D106" s="16" t="s">
         <v>582</v>
       </c>
-      <c r="D106" s="16" t="s">
+      <c r="E106" s="16" t="s">
         <v>583</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="F106" s="20" t="s">
         <v>584</v>
-      </c>
-      <c r="F106" s="20" t="s">
-        <v>585</v>
       </c>
       <c r="G106" s="17"/>
       <c r="H106" s="19" t="str">
@@ -6635,22 +6635,22 @@
     </row>
     <row r="107" spans="1:12" ht="15.75" customHeight="1">
       <c r="A107" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="C107" s="19" t="s">
         <v>586</v>
       </c>
-      <c r="B107" s="19" t="s">
-        <v>575</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>587</v>
-      </c>
       <c r="D107" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="E107" s="16" t="s">
         <v>577</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="F107" s="20" t="s">
         <v>578</v>
-      </c>
-      <c r="F107" s="20" t="s">
-        <v>579</v>
       </c>
       <c r="G107" s="17"/>
       <c r="H107" s="19" t="str">
@@ -6676,22 +6676,22 @@
     </row>
     <row r="108" spans="1:12" ht="15.75" customHeight="1">
       <c r="A108" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="B108" s="19" t="s">
         <v>588</v>
       </c>
-      <c r="B108" s="19" t="s">
+      <c r="C108" s="19" t="s">
         <v>589</v>
       </c>
-      <c r="C108" s="19" t="s">
+      <c r="D108" s="16" t="s">
         <v>590</v>
       </c>
-      <c r="D108" s="16" t="s">
+      <c r="E108" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="F108" s="20" t="s">
         <v>592</v>
-      </c>
-      <c r="F108" s="20" t="s">
-        <v>593</v>
       </c>
       <c r="G108" s="17"/>
       <c r="H108" s="19" t="str">
@@ -6717,22 +6717,22 @@
     </row>
     <row r="109" spans="1:12" ht="15.75" customHeight="1">
       <c r="A109" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="B109" s="19" t="s">
         <v>594</v>
       </c>
-      <c r="B109" s="19" t="s">
+      <c r="C109" s="19" t="s">
         <v>595</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="D109" s="16" t="s">
         <v>596</v>
       </c>
-      <c r="D109" s="16" t="s">
+      <c r="E109" s="16" t="s">
         <v>597</v>
       </c>
-      <c r="E109" s="16" t="s">
+      <c r="F109" s="20" t="s">
         <v>598</v>
-      </c>
-      <c r="F109" s="20" t="s">
-        <v>599</v>
       </c>
       <c r="G109" s="17"/>
       <c r="H109" s="19" t="str">
@@ -6758,22 +6758,22 @@
     </row>
     <row r="110" spans="1:12" ht="15.75" customHeight="1">
       <c r="A110" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="B110" s="19" t="s">
         <v>600</v>
       </c>
-      <c r="B110" s="19" t="s">
+      <c r="C110" s="19" t="s">
         <v>601</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="D110" s="16" t="s">
         <v>602</v>
       </c>
-      <c r="D110" s="16" t="s">
+      <c r="E110" s="16" t="s">
         <v>603</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="F110" s="20" t="s">
         <v>604</v>
-      </c>
-      <c r="F110" s="20" t="s">
-        <v>605</v>
       </c>
       <c r="G110" s="17"/>
       <c r="H110" s="19" t="str">
@@ -6799,22 +6799,22 @@
     </row>
     <row r="111" spans="1:12" ht="15.75" customHeight="1">
       <c r="A111" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="B111" s="19" t="s">
         <v>606</v>
       </c>
-      <c r="B111" s="19" t="s">
+      <c r="C111" s="19" t="s">
         <v>607</v>
       </c>
-      <c r="C111" s="19" t="s">
+      <c r="D111" s="16" t="s">
         <v>608</v>
       </c>
-      <c r="D111" s="16" t="s">
+      <c r="E111" s="16" t="s">
         <v>609</v>
       </c>
-      <c r="E111" s="16" t="s">
+      <c r="F111" s="20" t="s">
         <v>610</v>
-      </c>
-      <c r="F111" s="20" t="s">
-        <v>611</v>
       </c>
       <c r="G111" s="17"/>
       <c r="H111" s="19" t="str">
@@ -6840,22 +6840,22 @@
     </row>
     <row r="112" spans="1:12" ht="15.75" customHeight="1">
       <c r="A112" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="B112" s="19" t="s">
         <v>612</v>
       </c>
-      <c r="B112" s="19" t="s">
+      <c r="C112" s="19" t="s">
         <v>613</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="D112" s="16" t="s">
         <v>614</v>
       </c>
-      <c r="D112" s="16" t="s">
+      <c r="E112" s="16" t="s">
         <v>615</v>
       </c>
-      <c r="E112" s="16" t="s">
+      <c r="F112" s="20" t="s">
         <v>616</v>
-      </c>
-      <c r="F112" s="20" t="s">
-        <v>617</v>
       </c>
       <c r="G112" s="17"/>
       <c r="H112" s="19" t="str">
@@ -6881,22 +6881,22 @@
     </row>
     <row r="113" spans="1:12" ht="15.75" customHeight="1">
       <c r="A113" s="25" t="s">
+        <v>617</v>
+      </c>
+      <c r="B113" s="19" t="s">
         <v>618</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="C113" s="19" t="s">
         <v>619</v>
       </c>
-      <c r="C113" s="19" t="s">
+      <c r="D113" s="16" t="s">
         <v>620</v>
       </c>
-      <c r="D113" s="16" t="s">
+      <c r="E113" s="16" t="s">
         <v>621</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="F113" s="20" t="s">
         <v>622</v>
-      </c>
-      <c r="F113" s="20" t="s">
-        <v>623</v>
       </c>
       <c r="G113" s="17"/>
       <c r="H113" s="19" t="str">
@@ -6922,22 +6922,22 @@
     </row>
     <row r="114" spans="1:12" ht="15.75" customHeight="1">
       <c r="A114" s="25" t="s">
+        <v>623</v>
+      </c>
+      <c r="B114" s="19" t="s">
         <v>624</v>
       </c>
-      <c r="B114" s="19" t="s">
+      <c r="C114" s="19" t="s">
         <v>625</v>
       </c>
-      <c r="C114" s="19" t="s">
+      <c r="D114" s="16" t="s">
         <v>626</v>
       </c>
-      <c r="D114" s="16" t="s">
+      <c r="E114" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="E114" s="16" t="s">
+      <c r="F114" s="20" t="s">
         <v>628</v>
-      </c>
-      <c r="F114" s="20" t="s">
-        <v>629</v>
       </c>
       <c r="G114" s="17"/>
       <c r="H114" s="19" t="str">
@@ -6963,22 +6963,22 @@
     </row>
     <row r="115" spans="1:12" ht="15.75" customHeight="1">
       <c r="A115" s="25" t="s">
+        <v>629</v>
+      </c>
+      <c r="B115" s="19" t="s">
         <v>630</v>
       </c>
-      <c r="B115" s="19" t="s">
+      <c r="C115" s="19" t="s">
         <v>631</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="D115" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="D115" s="16" t="s">
+      <c r="E115" s="16" t="s">
         <v>633</v>
       </c>
-      <c r="E115" s="16" t="s">
+      <c r="F115" s="20" t="s">
         <v>634</v>
-      </c>
-      <c r="F115" s="20" t="s">
-        <v>635</v>
       </c>
       <c r="G115" s="17"/>
       <c r="H115" s="19" t="str">
@@ -7004,22 +7004,22 @@
     </row>
     <row r="116" spans="1:12" ht="15.75" customHeight="1">
       <c r="A116" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="B116" s="19" t="s">
         <v>636</v>
       </c>
-      <c r="B116" s="19" t="s">
+      <c r="C116" s="19" t="s">
         <v>637</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="D116" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="D116" s="16" t="s">
+      <c r="E116" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="F116" s="20" t="s">
         <v>640</v>
-      </c>
-      <c r="F116" s="20" t="s">
-        <v>641</v>
       </c>
       <c r="G116" s="17"/>
       <c r="H116" s="19" t="str">
@@ -7045,22 +7045,22 @@
     </row>
     <row r="117" spans="1:12" ht="15.75" customHeight="1">
       <c r="A117" s="25" t="s">
+        <v>641</v>
+      </c>
+      <c r="B117" s="19" t="s">
         <v>642</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="C117" s="19" t="s">
         <v>643</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="D117" s="16" t="s">
         <v>644</v>
       </c>
-      <c r="D117" s="16" t="s">
+      <c r="E117" s="16" t="s">
         <v>645</v>
       </c>
-      <c r="E117" s="16" t="s">
+      <c r="F117" s="20" t="s">
         <v>646</v>
-      </c>
-      <c r="F117" s="20" t="s">
-        <v>647</v>
       </c>
       <c r="G117" s="17"/>
       <c r="H117" s="19" t="str">
@@ -7086,22 +7086,22 @@
     </row>
     <row r="118" spans="1:12" ht="15.75" customHeight="1">
       <c r="A118" s="25" t="s">
+        <v>647</v>
+      </c>
+      <c r="B118" s="19" t="s">
         <v>648</v>
       </c>
-      <c r="B118" s="19" t="s">
+      <c r="C118" s="19" t="s">
         <v>649</v>
       </c>
-      <c r="C118" s="19" t="s">
+      <c r="D118" s="16" t="s">
         <v>650</v>
       </c>
-      <c r="D118" s="16" t="s">
+      <c r="E118" s="16" t="s">
         <v>651</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="F118" s="20" t="s">
         <v>652</v>
-      </c>
-      <c r="F118" s="20" t="s">
-        <v>653</v>
       </c>
       <c r="G118" s="17"/>
       <c r="H118" s="19" t="str">
@@ -7127,22 +7127,22 @@
     </row>
     <row r="119" spans="1:12" ht="15.75" customHeight="1">
       <c r="A119" s="25" t="s">
+        <v>653</v>
+      </c>
+      <c r="B119" s="19" t="s">
         <v>654</v>
       </c>
-      <c r="B119" s="19" t="s">
+      <c r="C119" s="19" t="s">
         <v>655</v>
       </c>
-      <c r="C119" s="19" t="s">
+      <c r="D119" s="16" t="s">
         <v>656</v>
       </c>
-      <c r="D119" s="16" t="s">
+      <c r="E119" s="16" t="s">
         <v>657</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="F119" s="20" t="s">
         <v>658</v>
-      </c>
-      <c r="F119" s="20" t="s">
-        <v>659</v>
       </c>
       <c r="G119" s="17"/>
       <c r="H119" s="19" t="str">
@@ -7177,19 +7177,19 @@
       <c r="F120" s="16"/>
       <c r="G120" s="17"/>
       <c r="H120" s="19" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I120" s="21" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J120" s="19" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K120" s="21" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="L120" s="26" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="15.75" customHeight="1">
@@ -8112,6 +8112,15 @@
   </sheetData>
   <autoFilter ref="A1:M152"/>
   <customSheetViews>
+    <customSheetView guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:K150"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="67239803"/>
+        </ext>
+      </extLst>
+    </customSheetView>
     <customSheetView guid="{02F08554-2E03-4827-AA05-82E0997FBBA8}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:K150">
@@ -8233,15 +8242,6 @@
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="300842063"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{3A6F2CDC-256D-4CA7-B8B0-EE39CA0997D0}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:K150"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="67239803"/>
         </ext>
       </extLst>
     </customSheetView>

</xml_diff>